<commit_message>
change in excel and bur repareihon in config door
</commit_message>
<xml_diff>
--- a/VenusDoors/Content/Template.xlsx
+++ b/VenusDoors/Content/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Source\Repos\VenusDoor\VenusDoors\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B366ECF2-96D8-4CF5-9B25-9E198F0ED50A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C01853-BB3E-4A93-807D-776DEC1988D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{C1E6BC7E-2CEA-47FB-8242-88CAE3E7473C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C1E6BC7E-2CEA-47FB-8242-88CAE3E7473C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E094A8F-8980-4FA7-9735-0D648E41A6FE}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,9 +1844,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D24" xr:uid="{486A7E39-7B95-427A-A347-2F592D0F16ED}">
       <formula1>"Select,2.5,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{75DEAE83-8FA5-4B99-ABA6-89DFB71BF44F}">
-      <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral,Flat Panel Beaded"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24" xr:uid="{C1491FCC-971C-40BD-98BF-6C21AFE1D509}">
       <formula1>"Select,Knotty Alder,Maple,Poplar,Red Oak,Beech"</formula1>
     </dataValidation>
@@ -1855,6 +1852,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G24" xr:uid="{3AEB39C5-987F-4F63-ACB8-F20E3B96F0CC}">
       <formula1>"Select,Stain Grade,Paint Grade"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{0F8FDDB4-406E-4197-8283-8DE08EE87B16}">
+      <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios para la carga masiva
</commit_message>
<xml_diff>
--- a/VenusDoors/Content/Template.xlsx
+++ b/VenusDoors/Content/Template.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Source\Repos\VenusDoor\VenusDoors\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C01853-BB3E-4A93-807D-776DEC1988D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C1E6BC7E-2CEA-47FB-8242-88CAE3E7473C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="26">
   <si>
     <t>DoorStyle</t>
   </si>
@@ -93,12 +92,24 @@
   </si>
   <si>
     <t>Grade</t>
+  </si>
+  <si>
+    <t>DoorType</t>
+  </si>
+  <si>
+    <t>FingerPull</t>
+  </si>
+  <si>
+    <t>DoorOption</t>
+  </si>
+  <si>
+    <t>Overlay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,27 +454,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E094A8F-8980-4FA7-9735-0D648E41A6FE}">
-  <dimension ref="A1:R24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,55 +482,67 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -550,32 +573,44 @@
       <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>18</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -606,32 +641,44 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>5</v>
-      </c>
-      <c r="O3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>18</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -662,32 +709,44 @@
       <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
         <v>16</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>18</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -718,32 +777,44 @@
       <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>5</v>
-      </c>
-      <c r="O5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
         <v>16</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>18</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -774,32 +845,44 @@
       <c r="J6" t="s">
         <v>19</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>5</v>
-      </c>
-      <c r="O6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
         <v>16</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>18</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -830,32 +913,44 @@
       <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>5</v>
-      </c>
-      <c r="O7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="s">
         <v>16</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>18</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -886,32 +981,44 @@
       <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>5</v>
-      </c>
-      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8" t="s">
         <v>16</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>18</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -942,32 +1049,44 @@
       <c r="J9" t="s">
         <v>19</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
       </c>
       <c r="M9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>5</v>
-      </c>
-      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9" t="s">
         <v>16</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>18</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" t="s">
+        <v>19</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -998,32 +1117,44 @@
       <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
       </c>
       <c r="M10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>5</v>
-      </c>
-      <c r="O10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
         <v>16</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>18</v>
       </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" t="s">
+        <v>19</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1054,32 +1185,44 @@
       <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>5</v>
-      </c>
-      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="s">
         <v>16</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>17</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>18</v>
       </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1110,32 +1253,44 @@
       <c r="J12" t="s">
         <v>19</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>5</v>
-      </c>
-      <c r="O12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="s">
         <v>16</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>18</v>
       </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" t="s">
+        <v>19</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1166,32 +1321,44 @@
       <c r="J13" t="s">
         <v>19</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" t="s">
+        <v>19</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>5</v>
-      </c>
-      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13" t="s">
         <v>16</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>18</v>
       </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U13" t="s">
+        <v>19</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1222,32 +1389,44 @@
       <c r="J14" t="s">
         <v>19</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" t="s">
+        <v>19</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>5</v>
-      </c>
-      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="s">
         <v>16</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>18</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1278,32 +1457,44 @@
       <c r="J15" t="s">
         <v>19</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" t="s">
+        <v>19</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>5</v>
-      </c>
-      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="s">
         <v>16</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>17</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>18</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1334,32 +1525,44 @@
       <c r="J16" t="s">
         <v>19</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" t="s">
+        <v>19</v>
       </c>
       <c r="M16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>5</v>
-      </c>
-      <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16" t="s">
         <v>16</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>18</v>
       </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" t="s">
+        <v>19</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1390,32 +1593,44 @@
       <c r="J17" t="s">
         <v>19</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" t="s">
+        <v>19</v>
       </c>
       <c r="M17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>5</v>
-      </c>
-      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17" t="s">
         <v>16</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>18</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1446,32 +1661,44 @@
       <c r="J18" t="s">
         <v>19</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" t="s">
+        <v>19</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>5</v>
-      </c>
-      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+      <c r="Q18" t="s">
         <v>16</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>18</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1502,32 +1729,44 @@
       <c r="J19" t="s">
         <v>19</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
+      <c r="K19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" t="s">
+        <v>19</v>
       </c>
       <c r="M19">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>5</v>
-      </c>
-      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>5</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19" t="s">
         <v>16</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="S19" t="s">
         <v>18</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1558,32 +1797,44 @@
       <c r="J20" t="s">
         <v>19</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" t="s">
+        <v>19</v>
       </c>
       <c r="M20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>5</v>
-      </c>
-      <c r="O20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>5</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
+      </c>
+      <c r="Q20" t="s">
         <v>16</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>17</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
         <v>18</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" t="s">
+        <v>19</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1614,32 +1865,44 @@
       <c r="J21" t="s">
         <v>19</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
+      <c r="K21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" t="s">
+        <v>19</v>
       </c>
       <c r="M21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>5</v>
-      </c>
-      <c r="O21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>5</v>
+      </c>
+      <c r="Q21" t="s">
         <v>16</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="S21" t="s">
         <v>18</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" t="s">
+        <v>19</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1670,32 +1933,44 @@
       <c r="J22" t="s">
         <v>19</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
+      <c r="K22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" t="s">
+        <v>19</v>
       </c>
       <c r="M22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>5</v>
-      </c>
-      <c r="O22" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22" t="s">
         <v>16</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>17</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="S22" t="s">
         <v>18</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>19</v>
+      </c>
+      <c r="U22" t="s">
+        <v>19</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1726,32 +2001,44 @@
       <c r="J23" t="s">
         <v>19</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
+      <c r="K23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" t="s">
+        <v>19</v>
       </c>
       <c r="M23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>5</v>
-      </c>
-      <c r="O23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23" t="s">
         <v>16</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="S23" t="s">
         <v>18</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23" t="s">
+        <v>19</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1782,79 +2069,103 @@
       <c r="J24" t="s">
         <v>19</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
+      <c r="K24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" t="s">
+        <v>19</v>
       </c>
       <c r="M24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>5</v>
-      </c>
-      <c r="O24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24" t="s">
         <v>16</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="S24" t="s">
         <v>18</v>
       </c>
-      <c r="R24">
+      <c r="T24" t="s">
+        <v>19</v>
+      </c>
+      <c r="U24" t="s">
+        <v>19</v>
+      </c>
+      <c r="V24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M24" xr:uid="{2E0E7EB3-ED14-455E-8391-F1E9C93CC5BF}">
+  <dataValidations count="19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O24">
       <formula1>5</formula1>
       <formula2>42</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N24" xr:uid="{1D16C293-31FD-4D43-B15B-FE9180FB2450}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24">
       <formula1>5</formula1>
       <formula2>96</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24" xr:uid="{7529B31F-EA59-4939-8C94-B5073FDAAAC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S24">
       <formula1>"No Opening,Opening"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24" xr:uid="{D2FE3240-4CEA-4B9C-9B0A-E39FF136383A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R24">
       <formula1>"Select,Right,Left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O24" xr:uid="{23D16D88-A226-4F28-AC8F-B6CEB9946BE6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24">
       <formula1>"No Drill,Drill"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L24" xr:uid="{A86507AF-F8F1-4A79-948B-F7B9C533C62B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L24">
+      <formula1>"Select,Shaker22,Ogee,Reba,Shaker Goove"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K24">
+      <formula1>"Select,Finger Pull,Reba,Shaker,Litte Bone,Double Roman Ogee,Half Reba"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J24">
+      <formula1>"Select,Cope and Stick,Miter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G24">
+      <formula1>"Select,Raised Panel,Flat Panel,Flat Panel Beaded"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24">
+      <formula1>"Select,Knotty Alder,Maple,Poplar,Red Oak,Beech"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H24">
+      <formula1>"Select,Knotty Alder,Maple,Poplar,Red Oak,Beech,MDF"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I24">
+      <formula1>"Select,Stain Grade,Paint Grade"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24">
+      <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T24">
+      <formula1>"Select,Lazy Susan,Single,Pair"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U24">
+      <formula1>"Select,Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24">
+      <formula1>"Select,Door,Drawer,Back Panel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24">
+      <formula1>"Select,Insert Door Type,Overlay Door Type"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M24 N2:N24">
       <formula1>"0,1,2,3,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J24" xr:uid="{FBE1529A-2A18-425A-B487-625FE61316E0}">
-      <formula1>"Select,Shaker22,Ogee,Reba,Shaker Goove"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I24" xr:uid="{66A7C49A-8C1E-41A3-9FCB-8D87E69C9442}">
-      <formula1>"Select,Finger Pull,Reba,Shaker,Litte Bone,Double Roman Ogee,Half Reba"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H24" xr:uid="{292C55CC-8D1A-4B1F-A5D9-547859819CB6}">
-      <formula1>"Select,Cope and Stick,Miter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E24" xr:uid="{AB08705D-9733-4F0E-9260-2F577C059C03}">
-      <formula1>"Select,Raised Panel,Flat Panel,Flat Panel Beaded"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D24" xr:uid="{486A7E39-7B95-427A-A347-2F592D0F16ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E24 F2:F24">
       <formula1>"Select,2.5,3"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24" xr:uid="{C1491FCC-971C-40BD-98BF-6C21AFE1D509}">
-      <formula1>"Select,Knotty Alder,Maple,Poplar,Red Oak,Beech"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F24" xr:uid="{2CA6D0A2-8D22-475B-8D0C-81191A52DA19}">
-      <formula1>"Select,Knotty Alder,Maple,Poplar,Red Oak,Beech,MDF"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G24" xr:uid="{3AEB39C5-987F-4F63-ACB8-F20E3B96F0CC}">
-      <formula1>"Select,Stain Grade,Paint Grade"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{0F8FDDB4-406E-4197-8283-8DE08EE87B16}">
-      <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1863,7 +2174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7396866-452F-4E66-80CC-1D50ABA19EDF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1894,7 +2205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194DFBE7-8F0D-45A6-BB21-7D204C723915}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
combo decimales en fracciones
</commit_message>
<xml_diff>
--- a/VenusDoors/Content/Template.xlsx
+++ b/VenusDoors/Content/Template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="28">
   <si>
     <t>DoorStyle</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Overlay</t>
+  </si>
+  <si>
+    <t>WidthDecimal</t>
+  </si>
+  <si>
+    <t>HeightDecimal</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,12 +475,15 @@
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,28 +530,34 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -588,29 +603,35 @@
       <c r="O2">
         <v>5</v>
       </c>
-      <c r="P2">
-        <v>5</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2">
+      <c r="V2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -656,29 +677,35 @@
       <c r="O3">
         <v>5</v>
       </c>
-      <c r="P3">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="s">
         <v>16</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>17</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>18</v>
       </c>
-      <c r="T3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -724,29 +751,35 @@
       <c r="O4">
         <v>5</v>
       </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>17</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>18</v>
       </c>
-      <c r="T4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -792,29 +825,35 @@
       <c r="O5">
         <v>5</v>
       </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
         <v>16</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>17</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>18</v>
       </c>
-      <c r="T5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" t="s">
+        <v>19</v>
+      </c>
+      <c r="X5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -860,29 +899,35 @@
       <c r="O6">
         <v>5</v>
       </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" t="s">
         <v>16</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>17</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>18</v>
       </c>
-      <c r="T6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -928,29 +973,35 @@
       <c r="O7">
         <v>5</v>
       </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" t="s">
         <v>16</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>17</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>18</v>
       </c>
-      <c r="T7" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" t="s">
-        <v>19</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -996,29 +1047,35 @@
       <c r="O8">
         <v>5</v>
       </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" t="s">
         <v>16</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>17</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>18</v>
       </c>
-      <c r="T8" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>19</v>
+      </c>
+      <c r="W8" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1064,29 +1121,35 @@
       <c r="O9">
         <v>5</v>
       </c>
-      <c r="P9">
-        <v>5</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="P9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" t="s">
         <v>16</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>17</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>18</v>
       </c>
-      <c r="T9" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" t="s">
-        <v>19</v>
-      </c>
-      <c r="V9">
+      <c r="V9" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" t="s">
+        <v>19</v>
+      </c>
+      <c r="X9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1132,29 +1195,35 @@
       <c r="O10">
         <v>5</v>
       </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="P10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" t="s">
         <v>16</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>17</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>18</v>
       </c>
-      <c r="T10" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" t="s">
-        <v>19</v>
-      </c>
-      <c r="V10">
+      <c r="V10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" t="s">
+        <v>19</v>
+      </c>
+      <c r="X10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1200,29 +1269,35 @@
       <c r="O11">
         <v>5</v>
       </c>
-      <c r="P11">
-        <v>5</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" t="s">
         <v>16</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>17</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>18</v>
       </c>
-      <c r="T11" t="s">
-        <v>19</v>
-      </c>
-      <c r="U11" t="s">
-        <v>19</v>
-      </c>
-      <c r="V11">
+      <c r="V11" t="s">
+        <v>19</v>
+      </c>
+      <c r="W11" t="s">
+        <v>19</v>
+      </c>
+      <c r="X11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1268,29 +1343,35 @@
       <c r="O12">
         <v>5</v>
       </c>
-      <c r="P12">
-        <v>5</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="P12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="R12" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" t="s">
         <v>16</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>17</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>18</v>
       </c>
-      <c r="T12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12">
+      <c r="V12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" t="s">
+        <v>19</v>
+      </c>
+      <c r="X12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1336,29 +1417,35 @@
       <c r="O13">
         <v>5</v>
       </c>
-      <c r="P13">
-        <v>5</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="P13" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" t="s">
         <v>16</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>17</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>18</v>
       </c>
-      <c r="T13" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" t="s">
-        <v>19</v>
-      </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" t="s">
+        <v>19</v>
+      </c>
+      <c r="X13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1404,29 +1491,35 @@
       <c r="O14">
         <v>5</v>
       </c>
-      <c r="P14">
-        <v>5</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="P14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14">
+        <v>5</v>
+      </c>
+      <c r="R14" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" t="s">
         <v>16</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>17</v>
       </c>
-      <c r="S14" t="s">
+      <c r="U14" t="s">
         <v>18</v>
       </c>
-      <c r="T14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U14" t="s">
-        <v>19</v>
-      </c>
-      <c r="V14">
+      <c r="V14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W14" t="s">
+        <v>19</v>
+      </c>
+      <c r="X14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1472,29 +1565,35 @@
       <c r="O15">
         <v>5</v>
       </c>
-      <c r="P15">
-        <v>5</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="P15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" t="s">
         <v>16</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>17</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>18</v>
       </c>
-      <c r="T15" t="s">
-        <v>19</v>
-      </c>
-      <c r="U15" t="s">
-        <v>19</v>
-      </c>
-      <c r="V15">
+      <c r="V15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1540,29 +1639,35 @@
       <c r="O16">
         <v>5</v>
       </c>
-      <c r="P16">
-        <v>5</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="P16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
         <v>16</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>17</v>
       </c>
-      <c r="S16" t="s">
+      <c r="U16" t="s">
         <v>18</v>
       </c>
-      <c r="T16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U16" t="s">
-        <v>19</v>
-      </c>
-      <c r="V16">
+      <c r="V16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W16" t="s">
+        <v>19</v>
+      </c>
+      <c r="X16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1608,29 +1713,35 @@
       <c r="O17">
         <v>5</v>
       </c>
-      <c r="P17">
-        <v>5</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="P17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
         <v>16</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>17</v>
       </c>
-      <c r="S17" t="s">
+      <c r="U17" t="s">
         <v>18</v>
       </c>
-      <c r="T17" t="s">
-        <v>19</v>
-      </c>
-      <c r="U17" t="s">
-        <v>19</v>
-      </c>
-      <c r="V17">
+      <c r="V17" t="s">
+        <v>19</v>
+      </c>
+      <c r="W17" t="s">
+        <v>19</v>
+      </c>
+      <c r="X17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1676,29 +1787,35 @@
       <c r="O18">
         <v>5</v>
       </c>
-      <c r="P18">
-        <v>5</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="P18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" t="s">
         <v>16</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>17</v>
       </c>
-      <c r="S18" t="s">
+      <c r="U18" t="s">
         <v>18</v>
       </c>
-      <c r="T18" t="s">
-        <v>19</v>
-      </c>
-      <c r="U18" t="s">
-        <v>19</v>
-      </c>
-      <c r="V18">
+      <c r="V18" t="s">
+        <v>19</v>
+      </c>
+      <c r="W18" t="s">
+        <v>19</v>
+      </c>
+      <c r="X18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1744,29 +1861,35 @@
       <c r="O19">
         <v>5</v>
       </c>
-      <c r="P19">
-        <v>5</v>
-      </c>
-      <c r="Q19" t="s">
+      <c r="P19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" t="s">
         <v>16</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>17</v>
       </c>
-      <c r="S19" t="s">
+      <c r="U19" t="s">
         <v>18</v>
       </c>
-      <c r="T19" t="s">
-        <v>19</v>
-      </c>
-      <c r="U19" t="s">
-        <v>19</v>
-      </c>
-      <c r="V19">
+      <c r="V19" t="s">
+        <v>19</v>
+      </c>
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1812,29 +1935,35 @@
       <c r="O20">
         <v>5</v>
       </c>
-      <c r="P20">
-        <v>5</v>
-      </c>
-      <c r="Q20" t="s">
+      <c r="P20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" t="s">
         <v>16</v>
       </c>
-      <c r="R20" t="s">
+      <c r="T20" t="s">
         <v>17</v>
       </c>
-      <c r="S20" t="s">
+      <c r="U20" t="s">
         <v>18</v>
       </c>
-      <c r="T20" t="s">
-        <v>19</v>
-      </c>
-      <c r="U20" t="s">
-        <v>19</v>
-      </c>
-      <c r="V20">
+      <c r="V20" t="s">
+        <v>19</v>
+      </c>
+      <c r="W20" t="s">
+        <v>19</v>
+      </c>
+      <c r="X20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1880,29 +2009,35 @@
       <c r="O21">
         <v>5</v>
       </c>
-      <c r="P21">
-        <v>5</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="P21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
         <v>16</v>
       </c>
-      <c r="R21" t="s">
+      <c r="T21" t="s">
         <v>17</v>
       </c>
-      <c r="S21" t="s">
+      <c r="U21" t="s">
         <v>18</v>
       </c>
-      <c r="T21" t="s">
-        <v>19</v>
-      </c>
-      <c r="U21" t="s">
-        <v>19</v>
-      </c>
-      <c r="V21">
+      <c r="V21" t="s">
+        <v>19</v>
+      </c>
+      <c r="W21" t="s">
+        <v>19</v>
+      </c>
+      <c r="X21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1948,29 +2083,35 @@
       <c r="O22">
         <v>5</v>
       </c>
-      <c r="P22">
-        <v>5</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="P22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22" t="s">
         <v>16</v>
       </c>
-      <c r="R22" t="s">
+      <c r="T22" t="s">
         <v>17</v>
       </c>
-      <c r="S22" t="s">
+      <c r="U22" t="s">
         <v>18</v>
       </c>
-      <c r="T22" t="s">
-        <v>19</v>
-      </c>
-      <c r="U22" t="s">
-        <v>19</v>
-      </c>
-      <c r="V22">
+      <c r="V22" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" t="s">
+        <v>19</v>
+      </c>
+      <c r="X22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2016,29 +2157,35 @@
       <c r="O23">
         <v>5</v>
       </c>
-      <c r="P23">
-        <v>5</v>
-      </c>
-      <c r="Q23" t="s">
+      <c r="P23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" t="s">
         <v>16</v>
       </c>
-      <c r="R23" t="s">
+      <c r="T23" t="s">
         <v>17</v>
       </c>
-      <c r="S23" t="s">
+      <c r="U23" t="s">
         <v>18</v>
       </c>
-      <c r="T23" t="s">
-        <v>19</v>
-      </c>
-      <c r="U23" t="s">
-        <v>19</v>
-      </c>
-      <c r="V23">
+      <c r="V23" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23" t="s">
+        <v>19</v>
+      </c>
+      <c r="X23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2084,45 +2231,51 @@
       <c r="O24">
         <v>5</v>
       </c>
-      <c r="P24">
-        <v>5</v>
-      </c>
-      <c r="Q24" t="s">
+      <c r="P24" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
+      <c r="R24" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" t="s">
         <v>16</v>
       </c>
-      <c r="R24" t="s">
+      <c r="T24" t="s">
         <v>17</v>
       </c>
-      <c r="S24" t="s">
+      <c r="U24" t="s">
         <v>18</v>
       </c>
-      <c r="T24" t="s">
-        <v>19</v>
-      </c>
-      <c r="U24" t="s">
-        <v>19</v>
-      </c>
-      <c r="V24">
+      <c r="V24" t="s">
+        <v>19</v>
+      </c>
+      <c r="W24" t="s">
+        <v>19</v>
+      </c>
+      <c r="X24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="19">
+  <dataValidations count="20">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O24">
       <formula1>5</formula1>
       <formula2>42</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24">
       <formula1>5</formula1>
       <formula2>96</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U24">
       <formula1>"No Opening,Opening"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T24">
       <formula1>"Select,Right,Left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S24">
       <formula1>"No Drill,Drill"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L24">
@@ -2149,10 +2302,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24">
       <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V24">
       <formula1>"Select,Lazy Susan,Single,Pair"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W24">
       <formula1>"Select,Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24">
@@ -2161,11 +2314,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24">
       <formula1>"Select,Insert Door Type,Overlay Door Type"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M24 N2:N24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:N24">
       <formula1>"0,1,2,3,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E24 F2:F24">
-      <formula1>"Select,2.5,3"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F24">
+      <formula1>"Select,2 1/2,3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24 R2:R24">
+      <formula1>"Select,0/16,1/16,1/8,3/16,1/4,5/16,3/8,7/16,1/2,9/16,5/8,11/16,3/4,13/16,7/8,15/16"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>